<commit_message>
v2.qmd: imported child count (19_20), visualizations, ODE home languages
</commit_message>
<xml_diff>
--- a/Data/ODE data v2.xlsx
+++ b/Data/ODE data v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E814D10F-FD95-0B4C-BD29-019BDF0CECCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D95604-2B52-F94C-AE05-9FBC9733A981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="500" windowWidth="22060" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="28480" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>Moved Out of State</t>
   </si>
   <si>
-    <t>Withdrawal By Parent (Or Guardian)</t>
-  </si>
-  <si>
     <t>Attempts To Contact Unsuccessful</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Withdrawal By Parent</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:O980"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:L43"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -528,10 +528,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>2</v>
@@ -555,15 +555,15 @@
         <v>3</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(D2:L2)</f>
@@ -596,17 +596,14 @@
       <c r="L2" s="6">
         <v>1</v>
       </c>
-      <c r="O2" s="7">
-        <f>75%*12</f>
-        <v>9</v>
-      </c>
+      <c r="O2" s="7"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="6">
         <f t="shared" ref="C3:C43" si="0">SUM(D3:L3)</f>
@@ -642,10 +639,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="6">
         <f t="shared" si="0"/>
@@ -681,10 +678,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
@@ -720,10 +717,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
@@ -759,10 +756,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
@@ -798,10 +795,10 @@
     </row>
     <row r="8" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
@@ -837,10 +834,10 @@
     </row>
     <row r="9" spans="1:15" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
@@ -876,10 +873,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
@@ -915,10 +912,10 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
@@ -954,10 +951,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
@@ -993,10 +990,10 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
@@ -1032,10 +1029,10 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
@@ -1071,10 +1068,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
@@ -1110,10 +1107,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
@@ -1149,10 +1146,10 @@
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
@@ -1188,10 +1185,10 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
@@ -1227,10 +1224,10 @@
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
@@ -1266,10 +1263,10 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
@@ -1305,10 +1302,10 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
@@ -1344,10 +1341,10 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
@@ -1383,10 +1380,10 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
@@ -1422,10 +1419,10 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
@@ -1461,10 +1458,10 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
@@ -1500,10 +1497,10 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
@@ -1539,10 +1536,10 @@
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="6">
         <f t="shared" si="0"/>
@@ -1578,10 +1575,10 @@
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" s="6">
         <f t="shared" si="0"/>
@@ -1617,10 +1614,10 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C29" s="6">
         <f t="shared" si="0"/>
@@ -1656,10 +1653,10 @@
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30" s="6">
         <f t="shared" si="0"/>
@@ -1695,10 +1692,10 @@
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" s="6">
         <f t="shared" si="0"/>
@@ -1734,10 +1731,10 @@
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C32" s="6">
         <f t="shared" si="0"/>
@@ -1773,10 +1770,10 @@
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" s="6">
         <f t="shared" si="0"/>
@@ -1812,10 +1809,10 @@
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C34" s="6">
         <f t="shared" si="0"/>
@@ -1851,10 +1848,10 @@
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" s="6">
         <f t="shared" si="0"/>
@@ -1890,10 +1887,10 @@
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C36" s="6">
         <f t="shared" si="0"/>
@@ -1929,10 +1926,10 @@
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C37" s="6">
         <f t="shared" si="0"/>
@@ -1968,10 +1965,10 @@
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C38" s="6">
         <f t="shared" si="0"/>
@@ -2007,10 +2004,10 @@
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C39" s="6">
         <f t="shared" si="0"/>
@@ -2046,10 +2043,10 @@
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C40" s="6">
         <f t="shared" si="0"/>
@@ -2085,10 +2082,10 @@
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C41" s="6">
         <f t="shared" si="0"/>
@@ -2124,10 +2121,10 @@
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C42" s="6">
         <f t="shared" si="0"/>
@@ -2163,10 +2160,10 @@
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C43" s="6">
         <f t="shared" si="0"/>
@@ -2214,7 +2211,7 @@
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -13477,15 +13474,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -13493,7 +13490,7 @@
         <v>1290</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -13501,7 +13498,7 @@
         <v>4260</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -13509,7 +13506,7 @@
         <v>3830</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -13517,7 +13514,7 @@
         <v>4800</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -13525,7 +13522,7 @@
         <v>860</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -13533,7 +13530,7 @@
         <v>4050</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -13541,7 +13538,7 @@
         <v>9999</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>